<commit_message>
Updating files and adding task_model.py and excel_handling.py
</commit_message>
<xml_diff>
--- a/task_manager_data.xlsx
+++ b/task_manager_data.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -516,6 +516,51 @@
       <c r="I2" t="inlineStr">
         <is>
           <t>wadawd</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>wesfaf</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>esafef</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>fasef</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>dfawef</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>efsef</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>seafsef</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>esafsefs</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>faefaf</t>
         </is>
       </c>
     </row>
@@ -530,7 +575,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -608,6 +653,72 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>aefs</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>dfasef</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>seafaes</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>esfasef</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>esafsefs</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>dtfdth</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>hfdth</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>hdfthg</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>dfthh</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>fhhddht</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>